<commit_message>
Feat : Excel 데이터 SO로 변환
</commit_message>
<xml_diff>
--- a/Assets/RawData/ItemDBSheet.xlsx
+++ b/Assets/RawData/ItemDBSheet.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity Work\Project_D\Assets\RawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AEEBC1A-6336-4CE4-AD42-468266551886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1685B6BF-3730-43D6-8F43-4AC23DA080F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{2AEBC651-332F-4C8D-B65D-23949F2277D1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2AEBC651-332F-4C8D-B65D-23949F2277D1}"/>
   </bookViews>
   <sheets>
-    <sheet name="테이블 명세표" sheetId="1" r:id="rId1"/>
-    <sheet name="Item_Table" sheetId="3" r:id="rId2"/>
-    <sheet name="Item_Grade" sheetId="7" r:id="rId3"/>
-    <sheet name="Item_Drop" sheetId="8" r:id="rId4"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
+    <sheet name="Item_Table" sheetId="3" r:id="rId1"/>
+    <sheet name="Item_Grade" sheetId="7" r:id="rId2"/>
+    <sheet name="Item_Drop" sheetId="8" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="테이블 명세표" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -659,8 +659,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7CA6A0F1-2006-44F2-BFBD-F16EC322364F}" name="표1" displayName="표1" ref="A1:J10" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J10" xr:uid="{7CA6A0F1-2006-44F2-BFBD-F16EC322364F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7CA6A0F1-2006-44F2-BFBD-F16EC322364F}" name="표1" displayName="표1" ref="A1:J2" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J2" xr:uid="{7CA6A0F1-2006-44F2-BFBD-F16EC322364F}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{C133476F-6A4D-4903-AB10-4ED2BF818DA5}" name="Id" dataDxfId="9"/>
     <tableColumn id="3" xr3:uid="{00019C6F-B17B-437F-8573-B68440833CAD}" name="Item_Name" dataDxfId="8"/>
@@ -993,6 +993,348 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5592392C-87E9-4C30-847D-A2C1E5C996FE}">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>10000001</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2">
+        <v>200</v>
+      </c>
+      <c r="E2">
+        <v>100</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E142078-3E9E-421E-95D2-E943B99AB92D}">
+  <dimension ref="A1:H14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H14">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{423DBB19-A89B-410F-B852-2D857E423C6C}">
+  <dimension ref="A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE19EB28-AE2E-4C4C-B24E-CC7D4F81DA9B}">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:L27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>10001</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>10002</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>10003</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>1001</v>
+      </c>
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="K9" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>1002</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>1003</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>1001</v>
+      </c>
+      <c r="C19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75767BC6-5953-440C-9975-DAB3B429A1BF}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:I35"/>
@@ -1379,386 +1721,4 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5592392C-87E9-4C30-847D-A2C1E5C996FE}">
-  <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:J10"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>10000001</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2">
-        <v>200</v>
-      </c>
-      <c r="E2">
-        <v>100</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>10000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>10000003</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>10000004</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>10000005</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>10000006</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>10000007</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>10000008</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>10000009</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E142078-3E9E-421E-95D2-E943B99AB92D}">
-  <dimension ref="A1:H14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H14">
-        <v>100</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{423DBB19-A89B-410F-B852-2D857E423C6C}">
-  <dimension ref="A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE19EB28-AE2E-4C4C-B24E-CC7D4F81DA9B}">
-  <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:L27"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>10001</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>10002</v>
-      </c>
-      <c r="B4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>10003</v>
-      </c>
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>1001</v>
-      </c>
-      <c r="B9" t="s">
-        <v>38</v>
-      </c>
-      <c r="K9" t="s">
-        <v>22</v>
-      </c>
-      <c r="L9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>1002</v>
-      </c>
-      <c r="B10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>1003</v>
-      </c>
-      <c r="B11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>2</v>
-      </c>
-      <c r="B16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>3</v>
-      </c>
-      <c r="B17" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B19">
-        <v>1001</v>
-      </c>
-      <c r="C19" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>